<commit_message>
Refactor exam/test services and controllers
Replaces ITestService with IExamService and updates DeThiController to use new exam service methods and DTOs. Removes legacy mixed test endpoints and related DTOs/validators, introduces new endpoints for generating exams and practice tests, and improves error handling and response structures. Updates question grouping logic in exam endpoints, aligns naming conventions, and removes obsolete code. Adds new DTOs and validators for exam configuration and joining, and updates related backend and frontend files to support the new exam flow and data structure.
</commit_message>
<xml_diff>
--- a/src/MsHuyenLC.Infrastructure/Templates/Excel/QuestionsTemplate.xlsx
+++ b/src/MsHuyenLC.Infrastructure/Templates/Excel/QuestionsTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\MsHuyenLC\src\MsHuyenLC.Infrastructure\Templates\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE5A8970-8658-4AC5-9666-015F6762E532}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7470FC7-BAC4-4571-8ECD-A1A2BEB9EF87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,24 +17,21 @@
     <sheet name="DanhMuc" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="CapDoList">DanhMuc!$A$12:$A$17</definedName>
-    <definedName name="DoKhoList">DanhMuc!$A$7:$A$9</definedName>
-    <definedName name="KyNangList">DanhMuc!$A$20:$A$22</definedName>
-    <definedName name="LoaiCauHoiList">DanhMuc!$A$2:$A$3</definedName>
+    <definedName name="CapDoList">DanhMuc!$A$9:$A$14</definedName>
+    <definedName name="DoKhoList">DanhMuc!$A$4:$A$6</definedName>
+    <definedName name="KyNangList">DanhMuc!$A$17:$A$21</definedName>
+    <definedName name="LoaiCauHoiList">DanhMuc!#REF!</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
   <si>
     <t>Nội dung</t>
   </si>
   <si>
-    <t>Loại câu hỏi</t>
-  </si>
-  <si>
     <t>Kỹ năng</t>
   </si>
   <si>
@@ -74,12 +71,6 @@
     <t>Giá trị</t>
   </si>
   <si>
-    <t>TracNghiem</t>
-  </si>
-  <si>
-    <t>TuLuan</t>
-  </si>
-  <si>
     <t>Dễ</t>
   </si>
   <si>
@@ -114,6 +105,12 @@
   </si>
   <si>
     <t>Viết</t>
+  </si>
+  <si>
+    <t>Từ vựng</t>
+  </si>
+  <si>
+    <t>Ngữ pháp</t>
   </si>
 </sst>
 </file>
@@ -453,15 +450,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N1"/>
+  <dimension ref="A1:M1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -501,22 +498,16 @@
       <c r="M1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
-        <v>13</v>
-      </c>
     </row>
   </sheetData>
-  <dataValidations count="4">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B2:B500" xr:uid="{00000000-0002-0000-0000-000000000000}">
-      <formula1>LoaiCauHoiList</formula1>
-    </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="D2:D500" xr:uid="{00000000-0002-0000-0000-000001000000}">
+  <dataValidations count="3">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C500" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>DoKhoList</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="E2:E500" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="D2:D500" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>CapDoList</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C500" xr:uid="{00000000-0002-0000-0000-000003000000}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B2:B500" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>KyNangList</formula1>
     </dataValidation>
   </dataValidations>
@@ -526,74 +517,76 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B22"/>
+  <dimension ref="A3:B21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-    </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7">
-        <v>0</v>
+        <v>16</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="B8" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B9">
-        <v>2</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>4</v>
-      </c>
-      <c r="B11" t="s">
-        <v>14</v>
+        <v>19</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -601,7 +594,7 @@
         <v>20</v>
       </c>
       <c r="B12">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -609,7 +602,7 @@
         <v>21</v>
       </c>
       <c r="B13">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -617,39 +610,39 @@
         <v>22</v>
       </c>
       <c r="B14">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>23</v>
-      </c>
-      <c r="B15">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>24</v>
-      </c>
-      <c r="B16">
-        <v>4</v>
+        <v>1</v>
+      </c>
+      <c r="B16" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B17">
-        <v>5</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19">
         <v>2</v>
-      </c>
-      <c r="B19" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -657,23 +650,15 @@
         <v>26</v>
       </c>
       <c r="B20">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>28</v>
-      </c>
-      <c r="B22">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>